<commit_message>
fix xlsx file (#119)
</commit_message>
<xml_diff>
--- a/slr/slr_articles.xlsx
+++ b/slr/slr_articles.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="1538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="1536">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -4625,12 +4625,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://ieeexplore.ieee.org/document/4299912</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service-oriented computing: Concepts, characteristics and directions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ieeexplore.ieee.org/document/1254461</t>
   </si>
   <si>
     <t xml:space="preserve">SOA anti-patterns </t>
@@ -14378,10 +14372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14536,38 +14530,28 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C14" s="12" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
         <v>1534</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="14" t="s">
         <v>1535</v>
       </c>
-      <c r="C14" s="12" t="n">
-        <v>3863</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1525</v>
-      </c>
-      <c r="C15" s="12" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>1536</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>1537</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="C15" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://link.springer.com/chapter/10.1007/978-3-642-02351-4_10"/>
@@ -14578,7 +14562,7 @@
     <hyperlink ref="B9" r:id="rId6" display="https://ieeexplore.ieee.org/document/5359597"/>
     <hyperlink ref="B10" r:id="rId7" display="https://ieeexplore.ieee.org/document/6671307"/>
     <hyperlink ref="B13" r:id="rId8" display="https://www.oreilly.com/library/view/microservices-antipatterns-and/9781492042716/ch01.html"/>
-    <hyperlink ref="B16" r:id="rId9" display="https://www.infoq.com/articles/SOA-anti-patterns"/>
+    <hyperlink ref="B15" r:id="rId9" display="https://www.infoq.com/articles/SOA-anti-patterns"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>